<commit_message>
new version, added ZM option
</commit_message>
<xml_diff>
--- a/test/template_results/generated vapor template (empty).xlsx
+++ b/test/template_results/generated vapor template (empty).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
   <si>
     <t>Overall Properties</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>Final Charge Pressure (after valve is closed, Pa)</t>
+  </si>
+  <si>
+    <t>Optional Analyses (add values to activate)</t>
+  </si>
+  <si>
+    <t>σ</t>
+  </si>
+  <si>
+    <t>Zimm Lundberg Analysis</t>
+  </si>
+  <si>
+    <t>Penetrant Liquid Phase Molar Volume (cm3/mol)</t>
   </si>
   <si>
     <t>---</t>
@@ -697,16 +709,25 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -723,16 +744,19 @@
         <v>0.5</v>
       </c>
       <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -752,16 +776,19 @@
         <v>0.0025</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -781,16 +808,16 @@
         <v>0.098002</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -810,16 +837,16 @@
         <v>0.023176</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -836,19 +863,19 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -871,16 +898,16 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -896,13 +923,13 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -924,46 +951,46 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="M11" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="O11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="P11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="S11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1025,1592 +1052,1592 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" t="s">
         <v>78</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>79</v>
       </c>
-      <c r="O1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" t="s">
-        <v>75</v>
-      </c>
       <c r="S1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="T1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="U1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA1" t="s">
         <v>78</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>79</v>
       </c>
-      <c r="Y1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>75</v>
-      </c>
       <c r="AC1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AD1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AE1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK1" t="s">
         <v>78</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AL1" t="s">
         <v>79</v>
       </c>
-      <c r="AI1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>75</v>
-      </c>
       <c r="AM1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AN1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AO1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AU1" t="s">
         <v>78</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AV1" t="s">
         <v>79</v>
       </c>
-      <c r="AS1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>75</v>
-      </c>
       <c r="AW1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AX1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AY1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BE1" t="s">
         <v>78</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BF1" t="s">
         <v>79</v>
       </c>
-      <c r="BC1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>75</v>
-      </c>
       <c r="BG1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="BH1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="BI1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BO1" t="s">
         <v>78</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BP1" t="s">
         <v>79</v>
       </c>
-      <c r="BM1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>75</v>
-      </c>
       <c r="BQ1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="BR1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="BS1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BY1" t="s">
         <v>78</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BZ1" t="s">
         <v>79</v>
       </c>
-      <c r="BW1" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>75</v>
-      </c>
       <c r="CA1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="CB1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="CC1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CI1" t="s">
         <v>78</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CJ1" t="s">
         <v>79</v>
       </c>
-      <c r="CG1" t="s">
-        <v>94</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>74</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>75</v>
-      </c>
       <c r="CK1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="CL1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="CM1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="CN1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="CQ1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:95">
       <c r="E2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="R2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="S2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="T2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="U2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Y2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AA2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AB2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AC2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AD2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AE2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AF2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AI2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AK2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AL2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AM2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AN2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AO2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AP2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AS2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AU2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AV2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AW2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AX2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AY2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AZ2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BC2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="BE2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BF2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BG2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BH2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BI2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BJ2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BM2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="BO2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BP2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BQ2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BR2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BS2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BT2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BW2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="BY2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BZ2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CA2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CB2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CC2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CD2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CG2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="CI2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CJ2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CK2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CL2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CM2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CN2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:95">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Q3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="R3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="S3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="T3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="U3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Y3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AA3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AB3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AC3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AD3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AE3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AF3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AI3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AK3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AL3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AM3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AN3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AO3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AP3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AS3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AU3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AV3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AW3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AX3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AY3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AZ3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BC3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="BE3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BF3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BG3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BH3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BI3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BJ3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BM3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="BO3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BP3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BQ3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BR3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BS3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BT3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BW3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="BY3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BZ3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CA3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CB3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CC3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CD3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CG3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="CI3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CJ3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CK3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CL3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CM3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CN3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:95">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="Q4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="R4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="T4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="U4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Y4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AA4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AB4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AC4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AD4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AE4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AF4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AI4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AK4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AL4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AM4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AN4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AO4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AP4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AS4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AU4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AV4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AW4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AX4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AY4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AZ4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BC4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="BE4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BF4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BG4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BH4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BI4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BJ4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BM4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="BO4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BP4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BQ4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BR4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BS4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BT4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BW4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="BY4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BZ4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CA4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CB4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CC4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CD4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CG4" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="CI4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CJ4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CK4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CL4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CM4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CN4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:95">
       <c r="B5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="Q5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="R5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="S5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="T5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="U5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Y5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AA5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AB5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AC5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AD5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AE5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AF5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AI5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AK5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AL5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AM5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AN5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AO5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AP5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AS5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AU5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AV5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AW5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AX5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AY5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AZ5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BC5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="BE5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BF5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BG5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BH5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BI5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BJ5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BM5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="BO5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BP5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BQ5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BR5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BS5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BT5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BW5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="BY5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BZ5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CA5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CB5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CC5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CD5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CG5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="CI5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CJ5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CK5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CL5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CM5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CN5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:95">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="R6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="S6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="T6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="U6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Y6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AA6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AB6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AC6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AD6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AE6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AF6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AI6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AK6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AL6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AM6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AN6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AO6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AP6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AS6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AU6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AV6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AW6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AX6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="AY6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AZ6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BC6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BE6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BF6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BG6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BH6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BI6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BJ6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BM6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BO6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BP6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BQ6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BR6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BS6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BT6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BW6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BY6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="BZ6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CA6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CB6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CC6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CD6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CG6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="CI6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CJ6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CK6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CL6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="CM6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CN6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:95">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>1000</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="R7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="S7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="T7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="U7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Y7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AA7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AB7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AC7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AD7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AE7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AF7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AI7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AK7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AL7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AM7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AN7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AO7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AP7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AS7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AU7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AV7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AW7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AX7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AY7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AZ7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BC7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="BE7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BF7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BG7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BH7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BI7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BJ7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BM7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="BO7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BP7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BQ7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BR7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BS7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BT7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BW7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="BY7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="BZ7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CA7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CB7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CC7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CD7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CG7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="CI7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CJ7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CK7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CL7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CM7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="CN7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:95">
       <c r="B8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="Y8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AI8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AS8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="BC8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="BM8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="BW8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="CG8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:95">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="M9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="N9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="O9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="P9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="W9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="X9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="Y9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="Z9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AG9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="AH9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="AI9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AJ9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AQ9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="AR9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="AS9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AT9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="BA9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BB9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BC9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="BD9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="BK9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BL9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BM9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="BN9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="BU9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BV9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BW9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="BX9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="CE9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="CF9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="CG9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="CH9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="CO9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="CP9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:95">
       <c r="E10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="Y10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AI10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AS10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="BC10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="BM10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="BW10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="CG10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:95">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="Z11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AJ11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AT11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="BD11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="BN11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="BX11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="CH11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added thermo factor functionality
</commit_message>
<xml_diff>
--- a/test/template_results/generated vapor template (empty).xlsx
+++ b/test/template_results/generated vapor template (empty).xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>Overall Properties</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>GAB Pred Err (CC/CC)</t>
+  </si>
+  <si>
+    <t>Thermodynamic Factor α</t>
+  </si>
+  <si>
+    <t>α err</t>
   </si>
   <si>
     <t>GAB (Cp)</t>
@@ -683,13 +689,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -730,7 +736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -759,7 +765,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -791,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -820,7 +826,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -837,7 +843,7 @@
         <v>0.023176</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -849,7 +855,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -866,7 +872,7 @@
         <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>40</v>
@@ -875,10 +881,10 @@
         <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -898,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
@@ -907,10 +913,10 @@
         <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -918,7 +924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -932,12 +938,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -992,38 +998,44 @@
       <c r="S11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="T11" t="s">
+        <v>54</v>
+      </c>
+      <c r="U11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:21">
       <c r="A16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:21">
       <c r="A17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:21">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1052,588 +1064,588 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" t="s">
+      <c r="S1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" t="s">
+      <c r="T1" t="s">
         <v>83</v>
       </c>
-      <c r="O1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AB1" t="s">
         <v>81</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AC1" t="s">
         <v>82</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AD1" t="s">
         <v>83</v>
       </c>
-      <c r="Y1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AL1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AM1" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AN1" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU1" t="s">
         <v>80</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AV1" t="s">
         <v>81</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AW1" t="s">
         <v>82</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AX1" t="s">
         <v>83</v>
       </c>
-      <c r="AS1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BE1" t="s">
         <v>80</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BF1" t="s">
         <v>81</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BG1" t="s">
         <v>82</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BH1" t="s">
         <v>83</v>
       </c>
-      <c r="BC1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BO1" t="s">
         <v>80</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BP1" t="s">
         <v>81</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BQ1" t="s">
         <v>82</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BR1" t="s">
         <v>83</v>
       </c>
-      <c r="BM1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>79</v>
-      </c>
-      <c r="BQ1" t="s">
+      <c r="BS1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BY1" t="s">
         <v>80</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BZ1" t="s">
         <v>81</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CA1" t="s">
         <v>82</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CB1" t="s">
         <v>83</v>
       </c>
-      <c r="BW1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>78</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CA1" t="s">
+      <c r="CC1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CI1" t="s">
         <v>80</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CJ1" t="s">
         <v>81</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CK1" t="s">
         <v>82</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CL1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>81</v>
-      </c>
       <c r="CM1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="CN1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="CQ1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:95">
       <c r="E2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Q2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Y2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AA2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AB2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AC2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AD2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AE2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AF2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AI2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AK2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AL2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AM2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AN2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AO2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AP2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AS2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AU2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AV2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AW2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AX2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AY2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AZ2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BC2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="BE2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BF2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BG2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BH2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BI2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BJ2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BM2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="BO2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BP2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BQ2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BR2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BS2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BT2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BW2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="BY2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BZ2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CA2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CB2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CC2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CD2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CG2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="CI2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CJ2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CK2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CL2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CM2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CN2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:95">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="Q3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Y3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AA3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AB3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AC3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AD3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AE3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AF3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AI3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AK3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AL3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AM3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AN3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AO3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AP3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AS3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AU3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AV3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AW3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AX3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AY3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AZ3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BC3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="BE3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BF3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BG3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BH3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BI3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BJ3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BM3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="BO3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BP3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BQ3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BR3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BS3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BT3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BW3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="BY3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BZ3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CA3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CB3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CC3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CD3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CG3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="CI3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CJ3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CK3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CL3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CM3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CN3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:95">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -1642,7 +1654,7 @@
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G4" t="s">
         <v>28</v>
@@ -1651,19 +1663,19 @@
         <v>28</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="Q4" t="s">
         <v>28</v>
@@ -1672,19 +1684,19 @@
         <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Y4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AA4" t="s">
         <v>28</v>
@@ -1693,19 +1705,19 @@
         <v>28</v>
       </c>
       <c r="AC4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AD4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AE4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AF4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AI4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AK4" t="s">
         <v>28</v>
@@ -1714,19 +1726,19 @@
         <v>28</v>
       </c>
       <c r="AM4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AN4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AO4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AP4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AS4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AU4" t="s">
         <v>28</v>
@@ -1735,19 +1747,19 @@
         <v>28</v>
       </c>
       <c r="AW4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AX4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AY4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AZ4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BC4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="BE4" t="s">
         <v>28</v>
@@ -1756,19 +1768,19 @@
         <v>28</v>
       </c>
       <c r="BG4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BH4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BI4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BJ4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BM4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="BO4" t="s">
         <v>28</v>
@@ -1777,19 +1789,19 @@
         <v>28</v>
       </c>
       <c r="BQ4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BR4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BS4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BT4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BW4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="BY4" t="s">
         <v>28</v>
@@ -1798,19 +1810,19 @@
         <v>28</v>
       </c>
       <c r="CA4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CB4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CC4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CD4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CG4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="CI4" t="s">
         <v>28</v>
@@ -1819,24 +1831,24 @@
         <v>28</v>
       </c>
       <c r="CK4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CL4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CM4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CN4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:95">
       <c r="B5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
         <v>28</v>
@@ -1845,19 +1857,19 @@
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q5" t="s">
         <v>28</v>
@@ -1866,19 +1878,19 @@
         <v>28</v>
       </c>
       <c r="S5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Y5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AA5" t="s">
         <v>28</v>
@@ -1887,19 +1899,19 @@
         <v>28</v>
       </c>
       <c r="AC5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AD5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AE5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AF5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AI5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AK5" t="s">
         <v>28</v>
@@ -1908,19 +1920,19 @@
         <v>28</v>
       </c>
       <c r="AM5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AN5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AO5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AP5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AS5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AU5" t="s">
         <v>28</v>
@@ -1929,19 +1941,19 @@
         <v>28</v>
       </c>
       <c r="AW5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AX5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AY5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AZ5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BC5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="BE5" t="s">
         <v>28</v>
@@ -1950,19 +1962,19 @@
         <v>28</v>
       </c>
       <c r="BG5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BH5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BI5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BJ5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BM5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="BO5" t="s">
         <v>28</v>
@@ -1971,19 +1983,19 @@
         <v>28</v>
       </c>
       <c r="BQ5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BR5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BS5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BT5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BW5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="BY5" t="s">
         <v>28</v>
@@ -1992,19 +2004,19 @@
         <v>28</v>
       </c>
       <c r="CA5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CB5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CC5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CD5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CG5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="CI5" t="s">
         <v>28</v>
@@ -2013,30 +2025,30 @@
         <v>28</v>
       </c>
       <c r="CK5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CL5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CM5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CN5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:95">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
@@ -2051,13 +2063,13 @@
         <v>28</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Q6" t="s">
         <v>28</v>
@@ -2072,13 +2084,13 @@
         <v>28</v>
       </c>
       <c r="U6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Y6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA6" t="s">
         <v>28</v>
@@ -2093,13 +2105,13 @@
         <v>28</v>
       </c>
       <c r="AE6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AF6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AI6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AK6" t="s">
         <v>28</v>
@@ -2114,13 +2126,13 @@
         <v>28</v>
       </c>
       <c r="AO6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AP6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AS6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AU6" t="s">
         <v>28</v>
@@ -2135,13 +2147,13 @@
         <v>28</v>
       </c>
       <c r="AY6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AZ6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BC6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="BE6" t="s">
         <v>28</v>
@@ -2156,13 +2168,13 @@
         <v>28</v>
       </c>
       <c r="BI6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BJ6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BM6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="BO6" t="s">
         <v>28</v>
@@ -2177,13 +2189,13 @@
         <v>28</v>
       </c>
       <c r="BS6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BT6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BW6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="BY6" t="s">
         <v>28</v>
@@ -2198,13 +2210,13 @@
         <v>28</v>
       </c>
       <c r="CC6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CD6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CG6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="CI6" t="s">
         <v>28</v>
@@ -2219,15 +2231,15 @@
         <v>28</v>
       </c>
       <c r="CM6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CN6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:95">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>1000</v>
@@ -2236,230 +2248,230 @@
         <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="O7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="Q7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Y7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AA7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AB7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AC7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AD7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AE7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AF7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AI7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AK7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AL7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AM7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AN7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AO7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AP7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AS7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AU7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AV7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AW7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AX7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AY7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AZ7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BC7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="BE7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BF7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BG7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BH7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BI7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BJ7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BM7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="BO7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BP7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BQ7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BR7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BS7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BT7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BW7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="BY7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="BZ7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CA7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CB7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CC7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CD7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CG7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="CI7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CJ7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CK7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CL7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CM7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="CN7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:95">
       <c r="B8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Y8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AI8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AS8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="BC8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="BM8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="BW8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="CG8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:95">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -2468,176 +2480,176 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M9" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" t="s">
         <v>87</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>88</v>
       </c>
-      <c r="O9" t="s">
-        <v>85</v>
-      </c>
-      <c r="P9" t="s">
-        <v>86</v>
-      </c>
       <c r="W9" t="s">
+        <v>89</v>
+      </c>
+      <c r="X9" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y9" t="s">
         <v>87</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Z9" t="s">
         <v>88</v>
       </c>
-      <c r="Y9" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>86</v>
-      </c>
       <c r="AG9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI9" t="s">
         <v>87</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AJ9" t="s">
         <v>88</v>
       </c>
-      <c r="AI9" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>86</v>
-      </c>
       <c r="AQ9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS9" t="s">
         <v>87</v>
       </c>
-      <c r="AR9" t="s">
+      <c r="AT9" t="s">
         <v>88</v>
       </c>
-      <c r="AS9" t="s">
-        <v>85</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>86</v>
-      </c>
       <c r="BA9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC9" t="s">
         <v>87</v>
       </c>
-      <c r="BB9" t="s">
+      <c r="BD9" t="s">
         <v>88</v>
       </c>
-      <c r="BC9" t="s">
-        <v>85</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>86</v>
-      </c>
       <c r="BK9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BL9" t="s">
+        <v>90</v>
+      </c>
+      <c r="BM9" t="s">
         <v>87</v>
       </c>
-      <c r="BL9" t="s">
+      <c r="BN9" t="s">
         <v>88</v>
       </c>
-      <c r="BM9" t="s">
-        <v>85</v>
-      </c>
-      <c r="BN9" t="s">
-        <v>86</v>
-      </c>
       <c r="BU9" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV9" t="s">
+        <v>90</v>
+      </c>
+      <c r="BW9" t="s">
         <v>87</v>
       </c>
-      <c r="BV9" t="s">
+      <c r="BX9" t="s">
         <v>88</v>
       </c>
-      <c r="BW9" t="s">
-        <v>85</v>
-      </c>
-      <c r="BX9" t="s">
-        <v>86</v>
-      </c>
       <c r="CE9" t="s">
+        <v>89</v>
+      </c>
+      <c r="CF9" t="s">
+        <v>90</v>
+      </c>
+      <c r="CG9" t="s">
         <v>87</v>
       </c>
-      <c r="CF9" t="s">
+      <c r="CH9" t="s">
         <v>88</v>
       </c>
-      <c r="CG9" t="s">
-        <v>85</v>
-      </c>
-      <c r="CH9" t="s">
-        <v>86</v>
-      </c>
       <c r="CO9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="CP9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:95">
       <c r="E10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="O10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Y10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AI10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AS10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="BC10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="BM10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="BW10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="CG10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:95">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Z11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AJ11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AT11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="BD11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="BN11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="BX11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="CH11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>